<commit_message>
Added function to easily repeat analysis functions for every player
</commit_message>
<xml_diff>
--- a/Example Spreadsheets/2017.12.22 1 Oh Heck Score Sheet.xlsx
+++ b/Example Spreadsheets/2017.12.22 1 Oh Heck Score Sheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianmcaulay/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianmcaulay/Programming/oh_heck_analysis/Example Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="E02935733946DB093E8A04C070C005AE4B403604" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -205,8 +204,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -457,9 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -752,97 +751,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
-    <col min="5" max="5" width="5.875" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="17.100000000000001" thickBot="1">
-      <c r="B4" s="21">
+    <row r="4" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20">
         <v>12</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="19">
+      <c r="C4" s="20"/>
+      <c r="D4" s="18">
         <f>IF(B4="","",IF(B4&gt;1,B4-1,""))</f>
         <v>11</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18">
         <f>IF(D4="","",IF(D4&gt;1,D4-1,""))</f>
         <v>10</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18">
         <f>IF(F4="","",IF(F4&gt;1,F4-1,""))</f>
         <v>9</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19">
+      <c r="I4" s="18"/>
+      <c r="J4" s="18">
         <f>IF(H4="","",IF(H4&gt;1,H4-1,""))</f>
         <v>8</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19">
+      <c r="K4" s="18"/>
+      <c r="L4" s="18">
         <f>IF(J4="","",IF(J4&gt;1,J4-1,""))</f>
         <v>7</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19">
+      <c r="M4" s="18"/>
+      <c r="N4" s="18">
         <f>IF(L4="","",IF(L4&gt;1,L4-1,""))</f>
         <v>6</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19">
+      <c r="O4" s="18"/>
+      <c r="P4" s="18">
         <f>IF(N4="","",IF(N4&gt;1,N4-1,""))</f>
         <v>5</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18">
         <f>IF(P4="","",IF(P4&gt;1,P4-1,""))</f>
         <v>4</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19">
+      <c r="S4" s="18"/>
+      <c r="T4" s="18">
         <f>IF(R4="","",IF(R4&gt;1,R4-1,""))</f>
         <v>3</v>
       </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19">
+      <c r="U4" s="18"/>
+      <c r="V4" s="18">
         <f>IF(T4="","",IF(T4&gt;1,T4-1,""))</f>
         <v>2</v>
       </c>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19">
+      <c r="W4" s="18"/>
+      <c r="X4" s="18">
         <f>IF(V4="","",IF(V4&gt;1,V4-1,""))</f>
         <v>1</v>
       </c>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19" t="str">
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18" t="str">
         <f>IF(X4="","",IF(X4&gt;1,X4-1,""))</f>
         <v/>
       </c>
-      <c r="AA4" s="19"/>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="A5" s="20" t="s">
+      <c r="AA4" s="18"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="8">
@@ -920,8 +919,8 @@
       <c r="Z5" s="17"/>
       <c r="AA5" s="17"/>
     </row>
-    <row r="6" spans="1:27" ht="17.100000000000001" thickBot="1">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="5"/>
       <c r="C6" s="13">
         <f>IF(C5 = "", "", IF(B5 = C5, C5 + 10, C5))</f>
@@ -985,8 +984,8 @@
       <c r="Z6" s="17"/>
       <c r="AA6" s="17"/>
     </row>
-    <row r="7" spans="1:27">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="8">
@@ -1064,8 +1063,8 @@
       <c r="Z7" s="17"/>
       <c r="AA7" s="17"/>
     </row>
-    <row r="8" spans="1:27" ht="17.100000000000001" thickBot="1">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
       <c r="B8" s="5"/>
       <c r="C8" s="13">
         <f>IF(C7 = "", "", IF(B7 = C7, C7 + 10, C7))</f>
@@ -1129,8 +1128,8 @@
       <c r="Z8" s="17"/>
       <c r="AA8" s="17"/>
     </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="8">
@@ -1208,8 +1207,8 @@
       <c r="Z9" s="17"/>
       <c r="AA9" s="17"/>
     </row>
-    <row r="10" spans="1:27" ht="17.100000000000001" thickBot="1">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
       <c r="B10" s="5"/>
       <c r="C10" s="13">
         <f>IF(C9 = "", "", IF(B9 = C9, C9 + 10, C9))</f>
@@ -1273,8 +1272,8 @@
       <c r="Z10" s="17"/>
       <c r="AA10" s="17"/>
     </row>
-    <row r="11" spans="1:27">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="8">
@@ -1352,8 +1351,8 @@
       <c r="Z11" s="17"/>
       <c r="AA11" s="17"/>
     </row>
-    <row r="12" spans="1:27" ht="17.100000000000001" thickBot="1">
-      <c r="A12" s="20"/>
+    <row r="12" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="15">
         <f>IF(C11 = "", "", IF(B11 = C11, C11 + 10, C11))</f>
@@ -1417,8 +1416,8 @@
       <c r="Z12" s="17"/>
       <c r="AA12" s="17"/>
     </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="18"/>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1446,8 +1445,8 @@
       <c r="Z13" s="17"/>
       <c r="AA13" s="17"/>
     </row>
-    <row r="14" spans="1:27">
-      <c r="A14" s="18"/>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -1475,8 +1474,8 @@
       <c r="Z14" s="17"/>
       <c r="AA14" s="17"/>
     </row>
-    <row r="15" spans="1:27">
-      <c r="A15" s="18"/>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" s="21"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -1504,8 +1503,8 @@
       <c r="Z15" s="17"/>
       <c r="AA15" s="17"/>
     </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="18"/>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" s="21"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -1533,8 +1532,8 @@
       <c r="Z16" s="17"/>
       <c r="AA16" s="17"/>
     </row>
-    <row r="17" spans="1:27">
-      <c r="A17" s="18"/>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -1562,8 +1561,8 @@
       <c r="Z17" s="17"/>
       <c r="AA17" s="17"/>
     </row>
-    <row r="18" spans="1:27">
-      <c r="A18" s="18"/>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" s="21"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -1591,8 +1590,8 @@
       <c r="Z18" s="17"/>
       <c r="AA18" s="17"/>
     </row>
-    <row r="19" spans="1:27">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1620,8 +1619,8 @@
       <c r="Z19" s="17"/>
       <c r="AA19" s="17"/>
     </row>
-    <row r="20" spans="1:27">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -1649,7 +1648,7 @@
       <c r="Z20" s="17"/>
       <c r="AA20" s="17"/>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1678,7 +1677,7 @@
       <c r="Z21" s="17"/>
       <c r="AA21" s="17"/>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1707,7 +1706,7 @@
       <c r="Z22" s="17"/>
       <c r="AA22" s="17"/>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1736,21 +1735,21 @@
       <c r="Z23" s="17"/>
       <c r="AA23" s="17"/>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1759,6 +1758,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="X4:Y4"/>
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -1775,36 +1779,31 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="X4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>12</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3-1</f>
         <v>11</v>
@@ -1901,7 +1900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B13" si="0">B4-1</f>
         <v>10</v>
@@ -1940,7 +1939,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1976,7 +1975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2009,7 +2008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2039,7 +2038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2066,7 +2065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2090,7 +2089,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2111,7 +2110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12">
         <f>B11-1</f>
         <v>3</v>
@@ -2129,7 +2128,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2144,7 +2143,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14">
         <f>B13-1</f>
         <v>1</v>

</xml_diff>